<commit_message>
TC up to 1.16
</commit_message>
<xml_diff>
--- a/TC/TC.xlsx
+++ b/TC/TC.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="256" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="280" uniqueCount="124">
   <si>
     <t>Test №</t>
   </si>
@@ -340,6 +340,57 @@
   </si>
   <si>
     <t>Откроется меню выбора приложения для открытия данного типа ссылок</t>
+  </si>
+  <si>
+    <t>Проверка сохраения данных, введённых в форму</t>
+  </si>
+  <si>
+    <t>Заполнить любую форму и отправить</t>
+  </si>
+  <si>
+    <t>На почтовый адрес администратора приходит сообщение с введёнными данными</t>
+  </si>
+  <si>
+    <t>Проверка открытия плаката фильма на полный экран</t>
+  </si>
+  <si>
+    <t>Находиться на странице с фильмом</t>
+  </si>
+  <si>
+    <t>Откроется фото в полноэкранном режиме</t>
+  </si>
+  <si>
+    <t>Проверка перехода браузера в полноэкранный режим</t>
+  </si>
+  <si>
+    <t>Находиться на странице с фильмом и открытой в полный экран обложкой</t>
+  </si>
+  <si>
+    <t>Браузер перейдёт в полноэкранный режим</t>
+  </si>
+  <si>
+    <t>Проверка выхода браузера из полноэкранного режима</t>
+  </si>
+  <si>
+    <t>Кликнуть ЛКМ на плакат</t>
+  </si>
+  <si>
+    <t>Кликнуть ЛКМ на кнопку, отвечающую за полноэкранный режим</t>
+  </si>
+  <si>
+    <t>Находиться на странице с фильмом и открытой в полный экран обложкой + полноэкранный режим браузера</t>
+  </si>
+  <si>
+    <t>Браузер выйдет из полноэкранного режима</t>
+  </si>
+  <si>
+    <t>Проверка работоспособности системы расшаривания фото в социальные сети</t>
+  </si>
+  <si>
+    <t>Редирект на выбранную соц. сеть</t>
+  </si>
+  <si>
+    <t>Кликнуть ЛКМ на Share-кнопку и выбрать соц.сеть</t>
   </si>
 </sst>
 </file>
@@ -846,7 +897,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="72">
+  <cellXfs count="79">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1026,6 +1077,27 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="10" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1345,10 +1417,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Z233"/>
+  <dimension ref="A1:Z248"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A218" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="L242" sqref="L242"/>
+    <sheetView tabSelected="1" topLeftCell="A223" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D252" sqref="D252"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -8308,11 +8380,11 @@
       <c r="K230" s="39"/>
       <c r="L230" s="39"/>
       <c r="M230" s="40"/>
-      <c r="N230" s="62"/>
-      <c r="O230" s="62"/>
-      <c r="P230" s="62"/>
-      <c r="Q230" s="62"/>
-      <c r="R230" s="62"/>
+      <c r="N230" s="69"/>
+      <c r="O230" s="69"/>
+      <c r="P230" s="69"/>
+      <c r="Q230" s="69"/>
+      <c r="R230" s="69"/>
       <c r="S230" s="49"/>
       <c r="T230" s="41"/>
       <c r="U230" s="41"/>
@@ -8342,14 +8414,14 @@
       <c r="K231" s="53"/>
       <c r="L231" s="53"/>
       <c r="M231" s="53"/>
-      <c r="N231" s="64" t="s">
+      <c r="N231" s="71" t="s">
         <v>106</v>
       </c>
-      <c r="O231" s="65"/>
-      <c r="P231" s="65"/>
-      <c r="Q231" s="65"/>
-      <c r="R231" s="66"/>
-      <c r="S231" s="60" t="s">
+      <c r="O231" s="72"/>
+      <c r="P231" s="72"/>
+      <c r="Q231" s="72"/>
+      <c r="R231" s="73"/>
+      <c r="S231" s="67" t="s">
         <v>41</v>
       </c>
       <c r="T231" s="47"/>
@@ -8374,12 +8446,12 @@
       <c r="K232" s="36"/>
       <c r="L232" s="36"/>
       <c r="M232" s="36"/>
-      <c r="N232" s="67"/>
-      <c r="O232" s="63"/>
-      <c r="P232" s="63"/>
-      <c r="Q232" s="63"/>
-      <c r="R232" s="68"/>
-      <c r="S232" s="61"/>
+      <c r="N232" s="74"/>
+      <c r="O232" s="70"/>
+      <c r="P232" s="70"/>
+      <c r="Q232" s="70"/>
+      <c r="R232" s="75"/>
+      <c r="S232" s="68"/>
       <c r="T232" s="41"/>
       <c r="U232" s="41"/>
       <c r="V232" s="41"/>
@@ -8402,12 +8474,12 @@
       <c r="K233" s="39"/>
       <c r="L233" s="39"/>
       <c r="M233" s="39"/>
-      <c r="N233" s="69"/>
-      <c r="O233" s="70"/>
-      <c r="P233" s="70"/>
-      <c r="Q233" s="70"/>
-      <c r="R233" s="71"/>
-      <c r="S233" s="61"/>
+      <c r="N233" s="76"/>
+      <c r="O233" s="77"/>
+      <c r="P233" s="77"/>
+      <c r="Q233" s="77"/>
+      <c r="R233" s="78"/>
+      <c r="S233" s="68"/>
       <c r="T233" s="41"/>
       <c r="U233" s="41"/>
       <c r="V233" s="41"/>
@@ -8416,10 +8488,528 @@
       <c r="Y233" s="9"/>
       <c r="Z233" s="9"/>
     </row>
+    <row r="234" spans="1:26" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A234" s="55">
+        <v>1.1299999999999999</v>
+      </c>
+      <c r="B234" s="5" t="s">
+        <v>107</v>
+      </c>
+      <c r="C234" s="5"/>
+      <c r="D234" s="5"/>
+      <c r="E234" s="56" t="s">
+        <v>108</v>
+      </c>
+      <c r="F234" s="11"/>
+      <c r="G234" s="11"/>
+      <c r="H234" s="11"/>
+      <c r="I234" s="11"/>
+      <c r="J234" s="52"/>
+      <c r="K234" s="53"/>
+      <c r="L234" s="53"/>
+      <c r="M234" s="53"/>
+      <c r="N234" s="71" t="s">
+        <v>109</v>
+      </c>
+      <c r="O234" s="72"/>
+      <c r="P234" s="72"/>
+      <c r="Q234" s="72"/>
+      <c r="R234" s="73"/>
+      <c r="S234" s="67" t="s">
+        <v>41</v>
+      </c>
+      <c r="T234" s="47"/>
+      <c r="U234" s="47"/>
+      <c r="V234" s="47"/>
+      <c r="W234" s="47"/>
+      <c r="X234" s="11"/>
+      <c r="Y234" s="11"/>
+      <c r="Z234" s="11"/>
+    </row>
+    <row r="235" spans="1:26" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A235" s="50"/>
+      <c r="B235" s="6"/>
+      <c r="C235" s="6"/>
+      <c r="D235" s="6"/>
+      <c r="E235" s="57"/>
+      <c r="F235" s="9"/>
+      <c r="G235" s="9"/>
+      <c r="H235" s="9"/>
+      <c r="I235" s="9"/>
+      <c r="J235" s="35"/>
+      <c r="K235" s="36"/>
+      <c r="L235" s="36"/>
+      <c r="M235" s="36"/>
+      <c r="N235" s="74"/>
+      <c r="O235" s="70"/>
+      <c r="P235" s="70"/>
+      <c r="Q235" s="70"/>
+      <c r="R235" s="75"/>
+      <c r="S235" s="68"/>
+      <c r="T235" s="41"/>
+      <c r="U235" s="41"/>
+      <c r="V235" s="41"/>
+      <c r="W235" s="41"/>
+      <c r="X235" s="9"/>
+      <c r="Y235" s="9"/>
+      <c r="Z235" s="9"/>
+    </row>
+    <row r="236" spans="1:26" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A236" s="51"/>
+      <c r="B236" s="7"/>
+      <c r="C236" s="7"/>
+      <c r="D236" s="7"/>
+      <c r="E236" s="57"/>
+      <c r="F236" s="9"/>
+      <c r="G236" s="9"/>
+      <c r="H236" s="9"/>
+      <c r="I236" s="9"/>
+      <c r="J236" s="38"/>
+      <c r="K236" s="39"/>
+      <c r="L236" s="39"/>
+      <c r="M236" s="39"/>
+      <c r="N236" s="76"/>
+      <c r="O236" s="77"/>
+      <c r="P236" s="77"/>
+      <c r="Q236" s="77"/>
+      <c r="R236" s="78"/>
+      <c r="S236" s="68"/>
+      <c r="T236" s="41"/>
+      <c r="U236" s="41"/>
+      <c r="V236" s="41"/>
+      <c r="W236" s="41"/>
+      <c r="X236" s="9"/>
+      <c r="Y236" s="9"/>
+      <c r="Z236" s="9"/>
+    </row>
+    <row r="237" spans="1:26" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A237" s="55">
+        <v>1.1399999999999999</v>
+      </c>
+      <c r="B237" s="5" t="s">
+        <v>110</v>
+      </c>
+      <c r="C237" s="5"/>
+      <c r="D237" s="5"/>
+      <c r="E237" s="56" t="s">
+        <v>117</v>
+      </c>
+      <c r="F237" s="11"/>
+      <c r="G237" s="11"/>
+      <c r="H237" s="11"/>
+      <c r="I237" s="11"/>
+      <c r="J237" s="52" t="s">
+        <v>111</v>
+      </c>
+      <c r="K237" s="53"/>
+      <c r="L237" s="53"/>
+      <c r="M237" s="53"/>
+      <c r="N237" s="71" t="s">
+        <v>112</v>
+      </c>
+      <c r="O237" s="72"/>
+      <c r="P237" s="72"/>
+      <c r="Q237" s="72"/>
+      <c r="R237" s="73"/>
+      <c r="S237" s="67" t="s">
+        <v>41</v>
+      </c>
+      <c r="T237" s="47"/>
+      <c r="U237" s="47"/>
+      <c r="V237" s="47"/>
+      <c r="W237" s="47"/>
+      <c r="X237" s="11"/>
+      <c r="Y237" s="11"/>
+      <c r="Z237" s="11"/>
+    </row>
+    <row r="238" spans="1:26" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A238" s="50"/>
+      <c r="B238" s="6"/>
+      <c r="C238" s="6"/>
+      <c r="D238" s="6"/>
+      <c r="E238" s="57"/>
+      <c r="F238" s="9"/>
+      <c r="G238" s="9"/>
+      <c r="H238" s="9"/>
+      <c r="I238" s="9"/>
+      <c r="J238" s="35"/>
+      <c r="K238" s="36"/>
+      <c r="L238" s="36"/>
+      <c r="M238" s="36"/>
+      <c r="N238" s="74"/>
+      <c r="O238" s="70"/>
+      <c r="P238" s="70"/>
+      <c r="Q238" s="70"/>
+      <c r="R238" s="75"/>
+      <c r="S238" s="68"/>
+      <c r="T238" s="41"/>
+      <c r="U238" s="41"/>
+      <c r="V238" s="41"/>
+      <c r="W238" s="41"/>
+      <c r="X238" s="9"/>
+      <c r="Y238" s="9"/>
+      <c r="Z238" s="9"/>
+    </row>
+    <row r="239" spans="1:26" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A239" s="51"/>
+      <c r="B239" s="7"/>
+      <c r="C239" s="7"/>
+      <c r="D239" s="7"/>
+      <c r="E239" s="57"/>
+      <c r="F239" s="9"/>
+      <c r="G239" s="9"/>
+      <c r="H239" s="9"/>
+      <c r="I239" s="9"/>
+      <c r="J239" s="38"/>
+      <c r="K239" s="39"/>
+      <c r="L239" s="39"/>
+      <c r="M239" s="39"/>
+      <c r="N239" s="76"/>
+      <c r="O239" s="77"/>
+      <c r="P239" s="77"/>
+      <c r="Q239" s="77"/>
+      <c r="R239" s="78"/>
+      <c r="S239" s="68"/>
+      <c r="T239" s="41"/>
+      <c r="U239" s="41"/>
+      <c r="V239" s="41"/>
+      <c r="W239" s="41"/>
+      <c r="X239" s="9"/>
+      <c r="Y239" s="9"/>
+      <c r="Z239" s="9"/>
+    </row>
+    <row r="240" spans="1:26" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A240" s="55">
+        <v>1.1499999999999999</v>
+      </c>
+      <c r="B240" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="C240" s="5"/>
+      <c r="D240" s="5"/>
+      <c r="E240" s="18" t="s">
+        <v>118</v>
+      </c>
+      <c r="F240" s="60"/>
+      <c r="G240" s="60"/>
+      <c r="H240" s="60"/>
+      <c r="I240" s="61"/>
+      <c r="J240" s="52" t="s">
+        <v>114</v>
+      </c>
+      <c r="K240" s="53"/>
+      <c r="L240" s="53"/>
+      <c r="M240" s="53"/>
+      <c r="N240" s="71" t="s">
+        <v>115</v>
+      </c>
+      <c r="O240" s="72"/>
+      <c r="P240" s="72"/>
+      <c r="Q240" s="72"/>
+      <c r="R240" s="73"/>
+      <c r="S240" s="67" t="s">
+        <v>41</v>
+      </c>
+      <c r="T240" s="47"/>
+      <c r="U240" s="47"/>
+      <c r="V240" s="47"/>
+      <c r="W240" s="47"/>
+      <c r="X240" s="11"/>
+      <c r="Y240" s="11"/>
+      <c r="Z240" s="11"/>
+    </row>
+    <row r="241" spans="1:26" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A241" s="50"/>
+      <c r="B241" s="6"/>
+      <c r="C241" s="6"/>
+      <c r="D241" s="6"/>
+      <c r="E241" s="62"/>
+      <c r="F241" s="63"/>
+      <c r="G241" s="63"/>
+      <c r="H241" s="63"/>
+      <c r="I241" s="64"/>
+      <c r="J241" s="35"/>
+      <c r="K241" s="36"/>
+      <c r="L241" s="36"/>
+      <c r="M241" s="36"/>
+      <c r="N241" s="74"/>
+      <c r="O241" s="70"/>
+      <c r="P241" s="70"/>
+      <c r="Q241" s="70"/>
+      <c r="R241" s="75"/>
+      <c r="S241" s="68"/>
+      <c r="T241" s="41"/>
+      <c r="U241" s="41"/>
+      <c r="V241" s="41"/>
+      <c r="W241" s="41"/>
+      <c r="X241" s="9"/>
+      <c r="Y241" s="9"/>
+      <c r="Z241" s="9"/>
+    </row>
+    <row r="242" spans="1:26" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A242" s="51"/>
+      <c r="B242" s="7"/>
+      <c r="C242" s="7"/>
+      <c r="D242" s="7"/>
+      <c r="E242" s="65"/>
+      <c r="F242" s="66"/>
+      <c r="G242" s="66"/>
+      <c r="H242" s="66"/>
+      <c r="I242" s="56"/>
+      <c r="J242" s="38"/>
+      <c r="K242" s="39"/>
+      <c r="L242" s="39"/>
+      <c r="M242" s="39"/>
+      <c r="N242" s="76"/>
+      <c r="O242" s="77"/>
+      <c r="P242" s="77"/>
+      <c r="Q242" s="77"/>
+      <c r="R242" s="78"/>
+      <c r="S242" s="68"/>
+      <c r="T242" s="41"/>
+      <c r="U242" s="41"/>
+      <c r="V242" s="41"/>
+      <c r="W242" s="41"/>
+      <c r="X242" s="9"/>
+      <c r="Y242" s="9"/>
+      <c r="Z242" s="9"/>
+    </row>
+    <row r="243" spans="1:26" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A243" s="55">
+        <v>1.1499999999999999</v>
+      </c>
+      <c r="B243" s="5" t="s">
+        <v>116</v>
+      </c>
+      <c r="C243" s="5"/>
+      <c r="D243" s="5"/>
+      <c r="E243" s="18" t="s">
+        <v>118</v>
+      </c>
+      <c r="F243" s="60"/>
+      <c r="G243" s="60"/>
+      <c r="H243" s="60"/>
+      <c r="I243" s="61"/>
+      <c r="J243" s="52" t="s">
+        <v>119</v>
+      </c>
+      <c r="K243" s="53"/>
+      <c r="L243" s="53"/>
+      <c r="M243" s="53"/>
+      <c r="N243" s="71" t="s">
+        <v>120</v>
+      </c>
+      <c r="O243" s="72"/>
+      <c r="P243" s="72"/>
+      <c r="Q243" s="72"/>
+      <c r="R243" s="73"/>
+      <c r="S243" s="67" t="s">
+        <v>41</v>
+      </c>
+      <c r="T243" s="47"/>
+      <c r="U243" s="47"/>
+      <c r="V243" s="47"/>
+      <c r="W243" s="47"/>
+      <c r="X243" s="11"/>
+      <c r="Y243" s="11"/>
+      <c r="Z243" s="11"/>
+    </row>
+    <row r="244" spans="1:26" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A244" s="50"/>
+      <c r="B244" s="6"/>
+      <c r="C244" s="6"/>
+      <c r="D244" s="6"/>
+      <c r="E244" s="62"/>
+      <c r="F244" s="63"/>
+      <c r="G244" s="63"/>
+      <c r="H244" s="63"/>
+      <c r="I244" s="64"/>
+      <c r="J244" s="35"/>
+      <c r="K244" s="36"/>
+      <c r="L244" s="36"/>
+      <c r="M244" s="36"/>
+      <c r="N244" s="74"/>
+      <c r="O244" s="70"/>
+      <c r="P244" s="70"/>
+      <c r="Q244" s="70"/>
+      <c r="R244" s="75"/>
+      <c r="S244" s="68"/>
+      <c r="T244" s="41"/>
+      <c r="U244" s="41"/>
+      <c r="V244" s="41"/>
+      <c r="W244" s="41"/>
+      <c r="X244" s="9"/>
+      <c r="Y244" s="9"/>
+      <c r="Z244" s="9"/>
+    </row>
+    <row r="245" spans="1:26" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A245" s="51"/>
+      <c r="B245" s="7"/>
+      <c r="C245" s="7"/>
+      <c r="D245" s="7"/>
+      <c r="E245" s="65"/>
+      <c r="F245" s="66"/>
+      <c r="G245" s="66"/>
+      <c r="H245" s="66"/>
+      <c r="I245" s="56"/>
+      <c r="J245" s="38"/>
+      <c r="K245" s="39"/>
+      <c r="L245" s="39"/>
+      <c r="M245" s="39"/>
+      <c r="N245" s="76"/>
+      <c r="O245" s="77"/>
+      <c r="P245" s="77"/>
+      <c r="Q245" s="77"/>
+      <c r="R245" s="78"/>
+      <c r="S245" s="68"/>
+      <c r="T245" s="41"/>
+      <c r="U245" s="41"/>
+      <c r="V245" s="41"/>
+      <c r="W245" s="41"/>
+      <c r="X245" s="9"/>
+      <c r="Y245" s="9"/>
+      <c r="Z245" s="9"/>
+    </row>
+    <row r="246" spans="1:26" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A246" s="55">
+        <v>1.1599999999999999</v>
+      </c>
+      <c r="B246" s="52" t="s">
+        <v>121</v>
+      </c>
+      <c r="C246" s="53"/>
+      <c r="D246" s="54"/>
+      <c r="E246" s="18" t="s">
+        <v>123</v>
+      </c>
+      <c r="F246" s="60"/>
+      <c r="G246" s="60"/>
+      <c r="H246" s="60"/>
+      <c r="I246" s="61"/>
+      <c r="J246" s="52" t="s">
+        <v>114</v>
+      </c>
+      <c r="K246" s="53"/>
+      <c r="L246" s="53"/>
+      <c r="M246" s="53"/>
+      <c r="N246" s="59" t="s">
+        <v>122</v>
+      </c>
+      <c r="O246" s="47"/>
+      <c r="P246" s="47"/>
+      <c r="Q246" s="47"/>
+      <c r="R246" s="47"/>
+      <c r="S246" s="48" t="s">
+        <v>41</v>
+      </c>
+      <c r="T246" s="47"/>
+      <c r="U246" s="47"/>
+      <c r="V246" s="47"/>
+      <c r="W246" s="47"/>
+      <c r="X246" s="11"/>
+      <c r="Y246" s="11"/>
+      <c r="Z246" s="11"/>
+    </row>
+    <row r="247" spans="1:26" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A247" s="50"/>
+      <c r="B247" s="35"/>
+      <c r="C247" s="36"/>
+      <c r="D247" s="37"/>
+      <c r="E247" s="62"/>
+      <c r="F247" s="63"/>
+      <c r="G247" s="63"/>
+      <c r="H247" s="63"/>
+      <c r="I247" s="64"/>
+      <c r="J247" s="35"/>
+      <c r="K247" s="36"/>
+      <c r="L247" s="36"/>
+      <c r="M247" s="36"/>
+      <c r="N247" s="41"/>
+      <c r="O247" s="41"/>
+      <c r="P247" s="41"/>
+      <c r="Q247" s="41"/>
+      <c r="R247" s="41"/>
+      <c r="S247" s="49"/>
+      <c r="T247" s="41"/>
+      <c r="U247" s="41"/>
+      <c r="V247" s="41"/>
+      <c r="W247" s="41"/>
+      <c r="X247" s="9"/>
+      <c r="Y247" s="9"/>
+      <c r="Z247" s="9"/>
+    </row>
+    <row r="248" spans="1:26" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A248" s="51"/>
+      <c r="B248" s="38"/>
+      <c r="C248" s="39"/>
+      <c r="D248" s="40"/>
+      <c r="E248" s="65"/>
+      <c r="F248" s="66"/>
+      <c r="G248" s="66"/>
+      <c r="H248" s="66"/>
+      <c r="I248" s="56"/>
+      <c r="J248" s="38"/>
+      <c r="K248" s="39"/>
+      <c r="L248" s="39"/>
+      <c r="M248" s="39"/>
+      <c r="N248" s="41"/>
+      <c r="O248" s="41"/>
+      <c r="P248" s="41"/>
+      <c r="Q248" s="41"/>
+      <c r="R248" s="41"/>
+      <c r="S248" s="49"/>
+      <c r="T248" s="41"/>
+      <c r="U248" s="41"/>
+      <c r="V248" s="41"/>
+      <c r="W248" s="41"/>
+      <c r="X248" s="9"/>
+      <c r="Y248" s="9"/>
+      <c r="Z248" s="9"/>
+    </row>
   </sheetData>
-  <mergeCells count="493">
+  <mergeCells count="533">
+    <mergeCell ref="A243:A245"/>
+    <mergeCell ref="B243:D245"/>
+    <mergeCell ref="B246:D248"/>
+    <mergeCell ref="A246:A248"/>
+    <mergeCell ref="A240:A242"/>
+    <mergeCell ref="B240:D242"/>
+    <mergeCell ref="E240:I242"/>
+    <mergeCell ref="J240:M242"/>
+    <mergeCell ref="N240:R242"/>
+    <mergeCell ref="S240:S242"/>
+    <mergeCell ref="T240:W242"/>
+    <mergeCell ref="X240:Z242"/>
+    <mergeCell ref="E243:I245"/>
+    <mergeCell ref="J243:M245"/>
+    <mergeCell ref="N243:R245"/>
+    <mergeCell ref="S243:S245"/>
+    <mergeCell ref="T243:W245"/>
+    <mergeCell ref="X243:Z245"/>
+    <mergeCell ref="E246:I248"/>
+    <mergeCell ref="J246:M248"/>
+    <mergeCell ref="N246:R248"/>
+    <mergeCell ref="S246:S248"/>
+    <mergeCell ref="T246:W248"/>
+    <mergeCell ref="X246:Z248"/>
+    <mergeCell ref="E237:I239"/>
+    <mergeCell ref="J237:M239"/>
+    <mergeCell ref="N237:R239"/>
+    <mergeCell ref="S237:S239"/>
+    <mergeCell ref="T237:W239"/>
+    <mergeCell ref="X237:Z239"/>
     <mergeCell ref="A231:A233"/>
     <mergeCell ref="B231:D233"/>
+    <mergeCell ref="A234:A236"/>
+    <mergeCell ref="B234:D236"/>
+    <mergeCell ref="A237:A239"/>
+    <mergeCell ref="B237:D239"/>
+    <mergeCell ref="X234:Z236"/>
+    <mergeCell ref="T234:W236"/>
+    <mergeCell ref="S234:S236"/>
+    <mergeCell ref="N234:R236"/>
+    <mergeCell ref="J234:M236"/>
+    <mergeCell ref="E234:I236"/>
     <mergeCell ref="X231:Z233"/>
     <mergeCell ref="T231:W233"/>
     <mergeCell ref="S231:S233"/>

</xml_diff>

<commit_message>
TC up to 1.20 & fully completed
</commit_message>
<xml_diff>
--- a/TC/TC.xlsx
+++ b/TC/TC.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="295" uniqueCount="134">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="374" uniqueCount="154">
   <si>
     <t>Test №</t>
   </si>
@@ -421,6 +421,66 @@
   </si>
   <si>
     <t>Переход на страницу с оформлением заказа</t>
+  </si>
+  <si>
+    <t>Проверка работоспособности ссылки на главную страницу в шапке</t>
+  </si>
+  <si>
+    <t>Нажать на логотип сайта в шапке</t>
+  </si>
+  <si>
+    <t>Откроется главная страница</t>
+  </si>
+  <si>
+    <t>Курсор должен быть не на этой ссылке</t>
+  </si>
+  <si>
+    <t>Курсор должен быть на этой ссылке</t>
+  </si>
+  <si>
+    <t>Ввести данные во всех обязательных формах</t>
+  </si>
+  <si>
+    <t>Ввести данные не во всех обязательных формах</t>
+  </si>
+  <si>
+    <t>Находиться на странице "О нас"</t>
+  </si>
+  <si>
+    <t>Находиться на странице "Оставить отзыв"</t>
+  </si>
+  <si>
+    <t>Находиться на странице с результатами поиска</t>
+  </si>
+  <si>
+    <t>Находиться на странице с формой написания отзыва</t>
+  </si>
+  <si>
+    <t>Находиться на странице "Фильмы"</t>
+  </si>
+  <si>
+    <t>Всплывающее окно</t>
+  </si>
+  <si>
+    <t>Находиться на странице с фильмами выбранного жанра</t>
+  </si>
+  <si>
+    <t>Страница с корзиной</t>
+  </si>
+  <si>
+    <t>Страница с корзиной, кликабельная кнопка</t>
+  </si>
+  <si>
+    <t>Страница с оформлением покупки</t>
+  </si>
+  <si>
+    <t>Наличие интернет-соединения и современного браузера</t>
+  </si>
+  <si>
+    <t>Открытая страница ввода пароля</t>
+  </si>
+  <si>
+    <t>Находиться на странице с любой формой</t>
   </si>
 </sst>
 </file>
@@ -927,7 +987,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="79">
+  <cellXfs count="80">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1082,6 +1142,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="2" fontId="3" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1447,10 +1510,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Z257"/>
+  <dimension ref="A1:Z260"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A232" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="N258" sqref="N258"/>
+    <sheetView tabSelected="1" topLeftCell="A219" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J237" sqref="J237:M239"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1920,7 +1983,9 @@
       <c r="G15" s="9"/>
       <c r="H15" s="9"/>
       <c r="I15" s="9"/>
-      <c r="J15" s="9"/>
+      <c r="J15" s="8" t="s">
+        <v>137</v>
+      </c>
       <c r="K15" s="9"/>
       <c r="L15" s="9"/>
       <c r="M15" s="9"/>
@@ -2010,7 +2075,9 @@
       <c r="G18" s="9"/>
       <c r="H18" s="9"/>
       <c r="I18" s="9"/>
-      <c r="J18" s="9"/>
+      <c r="J18" s="8" t="s">
+        <v>138</v>
+      </c>
       <c r="K18" s="9"/>
       <c r="L18" s="9"/>
       <c r="M18" s="9"/>
@@ -2100,7 +2167,9 @@
       <c r="G21" s="9"/>
       <c r="H21" s="9"/>
       <c r="I21" s="9"/>
-      <c r="J21" s="9"/>
+      <c r="J21" s="8" t="s">
+        <v>137</v>
+      </c>
       <c r="K21" s="9"/>
       <c r="L21" s="9"/>
       <c r="M21" s="9"/>
@@ -2190,7 +2259,9 @@
       <c r="G24" s="9"/>
       <c r="H24" s="9"/>
       <c r="I24" s="9"/>
-      <c r="J24" s="9"/>
+      <c r="J24" s="8" t="s">
+        <v>138</v>
+      </c>
       <c r="K24" s="9"/>
       <c r="L24" s="9"/>
       <c r="M24" s="9"/>
@@ -2280,7 +2351,9 @@
       <c r="G27" s="9"/>
       <c r="H27" s="9"/>
       <c r="I27" s="9"/>
-      <c r="J27" s="9"/>
+      <c r="J27" s="8" t="s">
+        <v>137</v>
+      </c>
       <c r="K27" s="9"/>
       <c r="L27" s="9"/>
       <c r="M27" s="9"/>
@@ -2370,7 +2443,9 @@
       <c r="G30" s="9"/>
       <c r="H30" s="9"/>
       <c r="I30" s="9"/>
-      <c r="J30" s="9"/>
+      <c r="J30" s="8" t="s">
+        <v>138</v>
+      </c>
       <c r="K30" s="9"/>
       <c r="L30" s="9"/>
       <c r="M30" s="9"/>
@@ -2464,7 +2539,9 @@
       <c r="G33" s="9"/>
       <c r="H33" s="9"/>
       <c r="I33" s="9"/>
-      <c r="J33" s="9"/>
+      <c r="J33" s="8" t="s">
+        <v>100</v>
+      </c>
       <c r="K33" s="9"/>
       <c r="L33" s="9"/>
       <c r="M33" s="9"/>
@@ -2554,7 +2631,9 @@
       <c r="G36" s="9"/>
       <c r="H36" s="9"/>
       <c r="I36" s="9"/>
-      <c r="J36" s="9"/>
+      <c r="J36" s="8" t="s">
+        <v>43</v>
+      </c>
       <c r="K36" s="9"/>
       <c r="L36" s="9"/>
       <c r="M36" s="9"/>
@@ -2644,7 +2723,9 @@
       <c r="G39" s="9"/>
       <c r="H39" s="9"/>
       <c r="I39" s="9"/>
-      <c r="J39" s="9"/>
+      <c r="J39" s="8" t="s">
+        <v>43</v>
+      </c>
       <c r="K39" s="9"/>
       <c r="L39" s="9"/>
       <c r="M39" s="9"/>
@@ -2734,7 +2815,9 @@
       <c r="G42" s="9"/>
       <c r="H42" s="9"/>
       <c r="I42" s="9"/>
-      <c r="J42" s="9"/>
+      <c r="J42" s="8" t="s">
+        <v>43</v>
+      </c>
       <c r="K42" s="9"/>
       <c r="L42" s="9"/>
       <c r="M42" s="9"/>
@@ -2824,7 +2907,9 @@
       <c r="G45" s="9"/>
       <c r="H45" s="9"/>
       <c r="I45" s="9"/>
-      <c r="J45" s="9"/>
+      <c r="J45" s="8" t="s">
+        <v>43</v>
+      </c>
       <c r="K45" s="9"/>
       <c r="L45" s="9"/>
       <c r="M45" s="9"/>
@@ -2914,7 +2999,9 @@
       <c r="G48" s="9"/>
       <c r="H48" s="9"/>
       <c r="I48" s="9"/>
-      <c r="J48" s="9"/>
+      <c r="J48" s="8" t="s">
+        <v>43</v>
+      </c>
       <c r="K48" s="9"/>
       <c r="L48" s="9"/>
       <c r="M48" s="9"/>
@@ -3004,7 +3091,9 @@
       <c r="G51" s="9"/>
       <c r="H51" s="9"/>
       <c r="I51" s="9"/>
-      <c r="J51" s="9"/>
+      <c r="J51" s="8" t="s">
+        <v>43</v>
+      </c>
       <c r="K51" s="9"/>
       <c r="L51" s="9"/>
       <c r="M51" s="9"/>
@@ -3094,7 +3183,9 @@
       <c r="G54" s="9"/>
       <c r="H54" s="9"/>
       <c r="I54" s="9"/>
-      <c r="J54" s="9"/>
+      <c r="J54" s="8" t="s">
+        <v>43</v>
+      </c>
       <c r="K54" s="9"/>
       <c r="L54" s="9"/>
       <c r="M54" s="9"/>
@@ -3184,7 +3275,9 @@
       <c r="G57" s="9"/>
       <c r="H57" s="9"/>
       <c r="I57" s="9"/>
-      <c r="J57" s="9"/>
+      <c r="J57" s="8" t="s">
+        <v>139</v>
+      </c>
       <c r="K57" s="9"/>
       <c r="L57" s="9"/>
       <c r="M57" s="9"/>
@@ -3262,7 +3355,7 @@
       <c r="Y59" s="9"/>
       <c r="Z59" s="9"/>
     </row>
-    <row r="60" spans="1:26" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:26" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A60" s="15">
         <v>1.4</v>
       </c>
@@ -3278,7 +3371,9 @@
       <c r="G60" s="9"/>
       <c r="H60" s="9"/>
       <c r="I60" s="9"/>
-      <c r="J60" s="9"/>
+      <c r="J60" s="8" t="s">
+        <v>100</v>
+      </c>
       <c r="K60" s="9"/>
       <c r="L60" s="9"/>
       <c r="M60" s="9"/>
@@ -3368,7 +3463,9 @@
       <c r="G63" s="9"/>
       <c r="H63" s="9"/>
       <c r="I63" s="9"/>
-      <c r="J63" s="9"/>
+      <c r="J63" s="8" t="s">
+        <v>43</v>
+      </c>
       <c r="K63" s="9"/>
       <c r="L63" s="9"/>
       <c r="M63" s="9"/>
@@ -3458,7 +3555,9 @@
       <c r="G66" s="9"/>
       <c r="H66" s="9"/>
       <c r="I66" s="9"/>
-      <c r="J66" s="9"/>
+      <c r="J66" s="8" t="s">
+        <v>43</v>
+      </c>
       <c r="K66" s="9"/>
       <c r="L66" s="9"/>
       <c r="M66" s="9"/>
@@ -3548,7 +3647,9 @@
       <c r="G69" s="9"/>
       <c r="H69" s="9"/>
       <c r="I69" s="9"/>
-      <c r="J69" s="9"/>
+      <c r="J69" s="8" t="s">
+        <v>43</v>
+      </c>
       <c r="K69" s="9"/>
       <c r="L69" s="9"/>
       <c r="M69" s="9"/>
@@ -3638,7 +3739,9 @@
       <c r="G72" s="9"/>
       <c r="H72" s="9"/>
       <c r="I72" s="9"/>
-      <c r="J72" s="9"/>
+      <c r="J72" s="8" t="s">
+        <v>43</v>
+      </c>
       <c r="K72" s="9"/>
       <c r="L72" s="9"/>
       <c r="M72" s="9"/>
@@ -3728,7 +3831,9 @@
       <c r="G75" s="9"/>
       <c r="H75" s="9"/>
       <c r="I75" s="9"/>
-      <c r="J75" s="9"/>
+      <c r="J75" s="8" t="s">
+        <v>43</v>
+      </c>
       <c r="K75" s="9"/>
       <c r="L75" s="9"/>
       <c r="M75" s="9"/>
@@ -3818,7 +3923,9 @@
       <c r="G78" s="9"/>
       <c r="H78" s="9"/>
       <c r="I78" s="9"/>
-      <c r="J78" s="9"/>
+      <c r="J78" s="8" t="s">
+        <v>43</v>
+      </c>
       <c r="K78" s="9"/>
       <c r="L78" s="9"/>
       <c r="M78" s="9"/>
@@ -3908,7 +4015,9 @@
       <c r="G81" s="9"/>
       <c r="H81" s="9"/>
       <c r="I81" s="9"/>
-      <c r="J81" s="9"/>
+      <c r="J81" s="8" t="s">
+        <v>43</v>
+      </c>
       <c r="K81" s="9"/>
       <c r="L81" s="9"/>
       <c r="M81" s="9"/>
@@ -3998,7 +4107,9 @@
       <c r="G84" s="9"/>
       <c r="H84" s="9"/>
       <c r="I84" s="9"/>
-      <c r="J84" s="9"/>
+      <c r="J84" s="8" t="s">
+        <v>140</v>
+      </c>
       <c r="K84" s="9"/>
       <c r="L84" s="9"/>
       <c r="M84" s="9"/>
@@ -4092,7 +4203,9 @@
       <c r="G87" s="9"/>
       <c r="H87" s="9"/>
       <c r="I87" s="9"/>
-      <c r="J87" s="9"/>
+      <c r="J87" s="8" t="s">
+        <v>100</v>
+      </c>
       <c r="K87" s="9"/>
       <c r="L87" s="9"/>
       <c r="M87" s="9"/>
@@ -4182,7 +4295,9 @@
       <c r="G90" s="9"/>
       <c r="H90" s="9"/>
       <c r="I90" s="9"/>
-      <c r="J90" s="9"/>
+      <c r="J90" s="8" t="s">
+        <v>141</v>
+      </c>
       <c r="K90" s="9"/>
       <c r="L90" s="9"/>
       <c r="M90" s="9"/>
@@ -4272,7 +4387,9 @@
       <c r="G93" s="9"/>
       <c r="H93" s="9"/>
       <c r="I93" s="9"/>
-      <c r="J93" s="9"/>
+      <c r="J93" s="8" t="s">
+        <v>142</v>
+      </c>
       <c r="K93" s="9"/>
       <c r="L93" s="9"/>
       <c r="M93" s="9"/>
@@ -4362,7 +4479,9 @@
       <c r="G96" s="9"/>
       <c r="H96" s="9"/>
       <c r="I96" s="9"/>
-      <c r="J96" s="9"/>
+      <c r="J96" s="8" t="s">
+        <v>142</v>
+      </c>
       <c r="K96" s="9"/>
       <c r="L96" s="9"/>
       <c r="M96" s="9"/>
@@ -4452,7 +4571,9 @@
       <c r="G99" s="9"/>
       <c r="H99" s="9"/>
       <c r="I99" s="9"/>
-      <c r="J99" s="9"/>
+      <c r="J99" s="8" t="s">
+        <v>142</v>
+      </c>
       <c r="K99" s="9"/>
       <c r="L99" s="9"/>
       <c r="M99" s="9"/>
@@ -4542,7 +4663,9 @@
       <c r="G102" s="9"/>
       <c r="H102" s="9"/>
       <c r="I102" s="9"/>
-      <c r="J102" s="9"/>
+      <c r="J102" s="8" t="s">
+        <v>142</v>
+      </c>
       <c r="K102" s="9"/>
       <c r="L102" s="9"/>
       <c r="M102" s="9"/>
@@ -4632,7 +4755,9 @@
       <c r="G105" s="9"/>
       <c r="H105" s="9"/>
       <c r="I105" s="9"/>
-      <c r="J105" s="9"/>
+      <c r="J105" s="8" t="s">
+        <v>142</v>
+      </c>
       <c r="K105" s="9"/>
       <c r="L105" s="9"/>
       <c r="M105" s="9"/>
@@ -4722,7 +4847,9 @@
       <c r="G108" s="9"/>
       <c r="H108" s="9"/>
       <c r="I108" s="9"/>
-      <c r="J108" s="9"/>
+      <c r="J108" s="8" t="s">
+        <v>139</v>
+      </c>
       <c r="K108" s="9"/>
       <c r="L108" s="9"/>
       <c r="M108" s="9"/>
@@ -4816,7 +4943,9 @@
       <c r="G111" s="11"/>
       <c r="H111" s="11"/>
       <c r="I111" s="11"/>
-      <c r="J111" s="9"/>
+      <c r="J111" s="8" t="s">
+        <v>100</v>
+      </c>
       <c r="K111" s="9"/>
       <c r="L111" s="9"/>
       <c r="M111" s="9"/>
@@ -4906,7 +5035,9 @@
       <c r="G114" s="9"/>
       <c r="H114" s="9"/>
       <c r="I114" s="9"/>
-      <c r="J114" s="9"/>
+      <c r="J114" s="8" t="s">
+        <v>42</v>
+      </c>
       <c r="K114" s="9"/>
       <c r="L114" s="9"/>
       <c r="M114" s="9"/>
@@ -4996,7 +5127,9 @@
       <c r="G117" s="9"/>
       <c r="H117" s="9"/>
       <c r="I117" s="9"/>
-      <c r="J117" s="9"/>
+      <c r="J117" s="8" t="s">
+        <v>42</v>
+      </c>
       <c r="K117" s="9"/>
       <c r="L117" s="9"/>
       <c r="M117" s="9"/>
@@ -5086,7 +5219,9 @@
       <c r="G120" s="9"/>
       <c r="H120" s="9"/>
       <c r="I120" s="9"/>
-      <c r="J120" s="9"/>
+      <c r="J120" s="8" t="s">
+        <v>42</v>
+      </c>
       <c r="K120" s="9"/>
       <c r="L120" s="9"/>
       <c r="M120" s="9"/>
@@ -5176,7 +5311,9 @@
       <c r="G123" s="9"/>
       <c r="H123" s="9"/>
       <c r="I123" s="9"/>
-      <c r="J123" s="9"/>
+      <c r="J123" s="8" t="s">
+        <v>139</v>
+      </c>
       <c r="K123" s="9"/>
       <c r="L123" s="9"/>
       <c r="M123" s="9"/>
@@ -5270,7 +5407,9 @@
       <c r="G126" s="9"/>
       <c r="H126" s="9"/>
       <c r="I126" s="9"/>
-      <c r="J126" s="9"/>
+      <c r="J126" s="8" t="s">
+        <v>100</v>
+      </c>
       <c r="K126" s="9"/>
       <c r="L126" s="9"/>
       <c r="M126" s="9"/>
@@ -5360,7 +5499,9 @@
       <c r="G129" s="9"/>
       <c r="H129" s="9"/>
       <c r="I129" s="9"/>
-      <c r="J129" s="9"/>
+      <c r="J129" s="8" t="s">
+        <v>100</v>
+      </c>
       <c r="K129" s="9"/>
       <c r="L129" s="9"/>
       <c r="M129" s="9"/>
@@ -5450,7 +5591,9 @@
       <c r="G132" s="9"/>
       <c r="H132" s="9"/>
       <c r="I132" s="9"/>
-      <c r="J132" s="9"/>
+      <c r="J132" s="8" t="s">
+        <v>143</v>
+      </c>
       <c r="K132" s="9"/>
       <c r="L132" s="9"/>
       <c r="M132" s="9"/>
@@ -5544,7 +5687,9 @@
       <c r="G135" s="9"/>
       <c r="H135" s="9"/>
       <c r="I135" s="9"/>
-      <c r="J135" s="9"/>
+      <c r="J135" s="8" t="s">
+        <v>100</v>
+      </c>
       <c r="K135" s="9"/>
       <c r="L135" s="9"/>
       <c r="M135" s="9"/>
@@ -5634,7 +5779,9 @@
       <c r="G138" s="9"/>
       <c r="H138" s="9"/>
       <c r="I138" s="9"/>
-      <c r="J138" s="9"/>
+      <c r="J138" s="8" t="s">
+        <v>100</v>
+      </c>
       <c r="K138" s="9"/>
       <c r="L138" s="9"/>
       <c r="M138" s="9"/>
@@ -5724,7 +5871,9 @@
       <c r="G141" s="9"/>
       <c r="H141" s="9"/>
       <c r="I141" s="9"/>
-      <c r="J141" s="9"/>
+      <c r="J141" s="8" t="s">
+        <v>143</v>
+      </c>
       <c r="K141" s="9"/>
       <c r="L141" s="9"/>
       <c r="M141" s="9"/>
@@ -5814,7 +5963,9 @@
       <c r="G144" s="9"/>
       <c r="H144" s="9"/>
       <c r="I144" s="9"/>
-      <c r="J144" s="9"/>
+      <c r="J144" s="8" t="s">
+        <v>111</v>
+      </c>
       <c r="K144" s="9"/>
       <c r="L144" s="9"/>
       <c r="M144" s="9"/>
@@ -5904,7 +6055,9 @@
       <c r="G147" s="9"/>
       <c r="H147" s="9"/>
       <c r="I147" s="9"/>
-      <c r="J147" s="9"/>
+      <c r="J147" s="8" t="s">
+        <v>144</v>
+      </c>
       <c r="K147" s="9"/>
       <c r="L147" s="9"/>
       <c r="M147" s="9"/>
@@ -5994,7 +6147,9 @@
       <c r="G150" s="9"/>
       <c r="H150" s="9"/>
       <c r="I150" s="9"/>
-      <c r="J150" s="9"/>
+      <c r="J150" s="8" t="s">
+        <v>144</v>
+      </c>
       <c r="K150" s="9"/>
       <c r="L150" s="9"/>
       <c r="M150" s="9"/>
@@ -6084,7 +6239,9 @@
       <c r="G153" s="9"/>
       <c r="H153" s="9"/>
       <c r="I153" s="9"/>
-      <c r="J153" s="9"/>
+      <c r="J153" s="8" t="s">
+        <v>144</v>
+      </c>
       <c r="K153" s="9"/>
       <c r="L153" s="9"/>
       <c r="M153" s="9"/>
@@ -6174,7 +6331,9 @@
       <c r="G156" s="9"/>
       <c r="H156" s="9"/>
       <c r="I156" s="9"/>
-      <c r="J156" s="9"/>
+      <c r="J156" s="8" t="s">
+        <v>144</v>
+      </c>
       <c r="K156" s="9"/>
       <c r="L156" s="9"/>
       <c r="M156" s="9"/>
@@ -6264,7 +6423,9 @@
       <c r="G159" s="9"/>
       <c r="H159" s="9"/>
       <c r="I159" s="9"/>
-      <c r="J159" s="9"/>
+      <c r="J159" s="8" t="s">
+        <v>144</v>
+      </c>
       <c r="K159" s="9"/>
       <c r="L159" s="9"/>
       <c r="M159" s="9"/>
@@ -6354,7 +6515,9 @@
       <c r="G162" s="9"/>
       <c r="H162" s="9"/>
       <c r="I162" s="9"/>
-      <c r="J162" s="9"/>
+      <c r="J162" s="8" t="s">
+        <v>144</v>
+      </c>
       <c r="K162" s="9"/>
       <c r="L162" s="9"/>
       <c r="M162" s="9"/>
@@ -6444,7 +6607,9 @@
       <c r="G165" s="9"/>
       <c r="H165" s="9"/>
       <c r="I165" s="9"/>
-      <c r="J165" s="9"/>
+      <c r="J165" s="8" t="s">
+        <v>144</v>
+      </c>
       <c r="K165" s="9"/>
       <c r="L165" s="9"/>
       <c r="M165" s="9"/>
@@ -6534,7 +6699,9 @@
       <c r="G168" s="9"/>
       <c r="H168" s="9"/>
       <c r="I168" s="9"/>
-      <c r="J168" s="9"/>
+      <c r="J168" s="8" t="s">
+        <v>139</v>
+      </c>
       <c r="K168" s="9"/>
       <c r="L168" s="9"/>
       <c r="M168" s="9"/>
@@ -6628,7 +6795,9 @@
       <c r="G171" s="11"/>
       <c r="H171" s="11"/>
       <c r="I171" s="11"/>
-      <c r="J171" s="9"/>
+      <c r="J171" s="8" t="s">
+        <v>100</v>
+      </c>
       <c r="K171" s="9"/>
       <c r="L171" s="9"/>
       <c r="M171" s="9"/>
@@ -6718,7 +6887,9 @@
       <c r="G174" s="9"/>
       <c r="H174" s="9"/>
       <c r="I174" s="9"/>
-      <c r="J174" s="9"/>
+      <c r="J174" s="8" t="s">
+        <v>145</v>
+      </c>
       <c r="K174" s="9"/>
       <c r="L174" s="9"/>
       <c r="M174" s="9"/>
@@ -6808,7 +6979,9 @@
       <c r="G177" s="9"/>
       <c r="H177" s="9"/>
       <c r="I177" s="9"/>
-      <c r="J177" s="9"/>
+      <c r="J177" s="8" t="s">
+        <v>147</v>
+      </c>
       <c r="K177" s="9"/>
       <c r="L177" s="9"/>
       <c r="M177" s="9"/>
@@ -6898,7 +7071,9 @@
       <c r="G180" s="9"/>
       <c r="H180" s="9"/>
       <c r="I180" s="9"/>
-      <c r="J180" s="9"/>
+      <c r="J180" s="8" t="s">
+        <v>146</v>
+      </c>
       <c r="K180" s="9"/>
       <c r="L180" s="9"/>
       <c r="M180" s="9"/>
@@ -6988,7 +7163,9 @@
       <c r="G183" s="9"/>
       <c r="H183" s="9"/>
       <c r="I183" s="9"/>
-      <c r="J183" s="9"/>
+      <c r="J183" s="8" t="s">
+        <v>147</v>
+      </c>
       <c r="K183" s="9"/>
       <c r="L183" s="9"/>
       <c r="M183" s="9"/>
@@ -7078,7 +7255,9 @@
       <c r="G186" s="9"/>
       <c r="H186" s="9"/>
       <c r="I186" s="9"/>
-      <c r="J186" s="9"/>
+      <c r="J186" s="8" t="s">
+        <v>146</v>
+      </c>
       <c r="K186" s="9"/>
       <c r="L186" s="9"/>
       <c r="M186" s="9"/>
@@ -7168,7 +7347,9 @@
       <c r="G189" s="9"/>
       <c r="H189" s="9"/>
       <c r="I189" s="9"/>
-      <c r="J189" s="9"/>
+      <c r="J189" s="8" t="s">
+        <v>148</v>
+      </c>
       <c r="K189" s="9"/>
       <c r="L189" s="9"/>
       <c r="M189" s="9"/>
@@ -7258,7 +7439,9 @@
       <c r="G192" s="9"/>
       <c r="H192" s="9"/>
       <c r="I192" s="9"/>
-      <c r="J192" s="9"/>
+      <c r="J192" s="8" t="s">
+        <v>149</v>
+      </c>
       <c r="K192" s="9"/>
       <c r="L192" s="9"/>
       <c r="M192" s="9"/>
@@ -7348,7 +7531,9 @@
       <c r="G195" s="9"/>
       <c r="H195" s="9"/>
       <c r="I195" s="9"/>
-      <c r="J195" s="9"/>
+      <c r="J195" s="8" t="s">
+        <v>150</v>
+      </c>
       <c r="K195" s="9"/>
       <c r="L195" s="9"/>
       <c r="M195" s="9"/>
@@ -7438,7 +7623,9 @@
       <c r="G198" s="9"/>
       <c r="H198" s="9"/>
       <c r="I198" s="9"/>
-      <c r="J198" s="9"/>
+      <c r="J198" s="8" t="s">
+        <v>150</v>
+      </c>
       <c r="K198" s="9"/>
       <c r="L198" s="9"/>
       <c r="M198" s="9"/>
@@ -7528,7 +7715,9 @@
       <c r="G201" s="9"/>
       <c r="H201" s="9"/>
       <c r="I201" s="9"/>
-      <c r="J201" s="9"/>
+      <c r="J201" s="8" t="s">
+        <v>150</v>
+      </c>
       <c r="K201" s="9"/>
       <c r="L201" s="9"/>
       <c r="M201" s="9"/>
@@ -7618,7 +7807,9 @@
       <c r="G204" s="9"/>
       <c r="H204" s="9"/>
       <c r="I204" s="9"/>
-      <c r="J204" s="9"/>
+      <c r="J204" s="8" t="s">
+        <v>150</v>
+      </c>
       <c r="K204" s="9"/>
       <c r="L204" s="9"/>
       <c r="M204" s="9"/>
@@ -7708,7 +7899,9 @@
       <c r="G207" s="9"/>
       <c r="H207" s="9"/>
       <c r="I207" s="9"/>
-      <c r="J207" s="9"/>
+      <c r="J207" s="8" t="s">
+        <v>150</v>
+      </c>
       <c r="K207" s="9"/>
       <c r="L207" s="9"/>
       <c r="M207" s="9"/>
@@ -7798,7 +7991,9 @@
       <c r="G210" s="9"/>
       <c r="H210" s="9"/>
       <c r="I210" s="9"/>
-      <c r="J210" s="9"/>
+      <c r="J210" s="8" t="s">
+        <v>150</v>
+      </c>
       <c r="K210" s="9"/>
       <c r="L210" s="9"/>
       <c r="M210" s="9"/>
@@ -7888,7 +8083,9 @@
       <c r="G213" s="9"/>
       <c r="H213" s="9"/>
       <c r="I213" s="9"/>
-      <c r="J213" s="9"/>
+      <c r="J213" s="8" t="s">
+        <v>150</v>
+      </c>
       <c r="K213" s="9"/>
       <c r="L213" s="9"/>
       <c r="M213" s="9"/>
@@ -7978,7 +8175,9 @@
       <c r="G216" s="9"/>
       <c r="H216" s="9"/>
       <c r="I216" s="9"/>
-      <c r="J216" s="9"/>
+      <c r="J216" s="8" t="s">
+        <v>139</v>
+      </c>
       <c r="K216" s="9"/>
       <c r="L216" s="9"/>
       <c r="M216" s="9"/>
@@ -8038,10 +8237,10 @@
       <c r="G218" s="9"/>
       <c r="H218" s="9"/>
       <c r="I218" s="9"/>
-      <c r="J218" s="43"/>
-      <c r="K218" s="43"/>
-      <c r="L218" s="43"/>
-      <c r="M218" s="43"/>
+      <c r="J218" s="9"/>
+      <c r="K218" s="9"/>
+      <c r="L218" s="9"/>
+      <c r="M218" s="9"/>
       <c r="N218" s="9"/>
       <c r="O218" s="9"/>
       <c r="P218" s="9"/>
@@ -8057,7 +8256,7 @@
       <c r="Z218" s="9"/>
     </row>
     <row r="219" spans="1:26" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A219" s="55">
+      <c r="A219" s="56">
         <v>1.1000000000000001</v>
       </c>
       <c r="B219" s="5" t="s">
@@ -8065,18 +8264,20 @@
       </c>
       <c r="C219" s="5"/>
       <c r="D219" s="5"/>
-      <c r="E219" s="56" t="s">
+      <c r="E219" s="57" t="s">
         <v>95</v>
       </c>
       <c r="F219" s="11"/>
       <c r="G219" s="11"/>
       <c r="H219" s="11"/>
       <c r="I219" s="11"/>
-      <c r="J219" s="52"/>
-      <c r="K219" s="53"/>
-      <c r="L219" s="53"/>
-      <c r="M219" s="54"/>
-      <c r="N219" s="59" t="s">
+      <c r="J219" s="53" t="s">
+        <v>151</v>
+      </c>
+      <c r="K219" s="54"/>
+      <c r="L219" s="54"/>
+      <c r="M219" s="55"/>
+      <c r="N219" s="60" t="s">
         <v>99</v>
       </c>
       <c r="O219" s="47"/>
@@ -8099,7 +8300,7 @@
       <c r="B220" s="6"/>
       <c r="C220" s="6"/>
       <c r="D220" s="6"/>
-      <c r="E220" s="57"/>
+      <c r="E220" s="58"/>
       <c r="F220" s="9"/>
       <c r="G220" s="9"/>
       <c r="H220" s="9"/>
@@ -8127,7 +8328,7 @@
       <c r="B221" s="6"/>
       <c r="C221" s="6"/>
       <c r="D221" s="6"/>
-      <c r="E221" s="57"/>
+      <c r="E221" s="58"/>
       <c r="F221" s="9"/>
       <c r="G221" s="9"/>
       <c r="H221" s="9"/>
@@ -8162,7 +8363,9 @@
       <c r="G222" s="24"/>
       <c r="H222" s="24"/>
       <c r="I222" s="24"/>
-      <c r="J222" s="8"/>
+      <c r="J222" s="8" t="s">
+        <v>152</v>
+      </c>
       <c r="K222" s="9"/>
       <c r="L222" s="9"/>
       <c r="M222" s="9"/>
@@ -8245,17 +8448,19 @@
       <c r="B225" s="6"/>
       <c r="C225" s="6"/>
       <c r="D225" s="6"/>
-      <c r="E225" s="58" t="s">
+      <c r="E225" s="59" t="s">
         <v>97</v>
       </c>
       <c r="F225" s="9"/>
       <c r="G225" s="9"/>
       <c r="H225" s="9"/>
       <c r="I225" s="9"/>
-      <c r="J225" s="28"/>
-      <c r="K225" s="19"/>
-      <c r="L225" s="19"/>
-      <c r="M225" s="29"/>
+      <c r="J225" s="8" t="s">
+        <v>152</v>
+      </c>
+      <c r="K225" s="9"/>
+      <c r="L225" s="9"/>
+      <c r="M225" s="9"/>
       <c r="N225" s="8" t="s">
         <v>98</v>
       </c>
@@ -8279,15 +8484,15 @@
       <c r="B226" s="6"/>
       <c r="C226" s="6"/>
       <c r="D226" s="6"/>
-      <c r="E226" s="57"/>
+      <c r="E226" s="58"/>
       <c r="F226" s="9"/>
       <c r="G226" s="9"/>
       <c r="H226" s="9"/>
       <c r="I226" s="9"/>
-      <c r="J226" s="20"/>
-      <c r="K226" s="21"/>
-      <c r="L226" s="21"/>
-      <c r="M226" s="30"/>
+      <c r="J226" s="9"/>
+      <c r="K226" s="9"/>
+      <c r="L226" s="9"/>
+      <c r="M226" s="9"/>
       <c r="N226" s="9"/>
       <c r="O226" s="9"/>
       <c r="P226" s="9"/>
@@ -8307,15 +8512,15 @@
       <c r="B227" s="7"/>
       <c r="C227" s="7"/>
       <c r="D227" s="7"/>
-      <c r="E227" s="57"/>
+      <c r="E227" s="58"/>
       <c r="F227" s="9"/>
       <c r="G227" s="9"/>
       <c r="H227" s="9"/>
       <c r="I227" s="9"/>
-      <c r="J227" s="22"/>
-      <c r="K227" s="23"/>
-      <c r="L227" s="23"/>
-      <c r="M227" s="31"/>
+      <c r="J227" s="9"/>
+      <c r="K227" s="9"/>
+      <c r="L227" s="9"/>
+      <c r="M227" s="9"/>
       <c r="N227" s="9"/>
       <c r="O227" s="9"/>
       <c r="P227" s="9"/>
@@ -8331,7 +8536,7 @@
       <c r="Z227" s="9"/>
     </row>
     <row r="228" spans="1:26" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A228" s="55">
+      <c r="A228" s="56">
         <v>1.1100000000000001</v>
       </c>
       <c r="B228" s="5" t="s">
@@ -8339,18 +8544,20 @@
       </c>
       <c r="C228" s="5"/>
       <c r="D228" s="5"/>
-      <c r="E228" s="56" t="s">
+      <c r="E228" s="57" t="s">
         <v>102</v>
       </c>
       <c r="F228" s="11"/>
       <c r="G228" s="11"/>
       <c r="H228" s="11"/>
       <c r="I228" s="11"/>
-      <c r="J228" s="52"/>
-      <c r="K228" s="53"/>
-      <c r="L228" s="53"/>
-      <c r="M228" s="54"/>
-      <c r="N228" s="59" t="s">
+      <c r="J228" s="53" t="s">
+        <v>100</v>
+      </c>
+      <c r="K228" s="54"/>
+      <c r="L228" s="54"/>
+      <c r="M228" s="55"/>
+      <c r="N228" s="60" t="s">
         <v>103</v>
       </c>
       <c r="O228" s="47"/>
@@ -8373,7 +8580,7 @@
       <c r="B229" s="6"/>
       <c r="C229" s="6"/>
       <c r="D229" s="6"/>
-      <c r="E229" s="57"/>
+      <c r="E229" s="58"/>
       <c r="F229" s="9"/>
       <c r="G229" s="9"/>
       <c r="H229" s="9"/>
@@ -8401,7 +8608,7 @@
       <c r="B230" s="7"/>
       <c r="C230" s="7"/>
       <c r="D230" s="7"/>
-      <c r="E230" s="57"/>
+      <c r="E230" s="58"/>
       <c r="F230" s="9"/>
       <c r="G230" s="9"/>
       <c r="H230" s="9"/>
@@ -8410,11 +8617,11 @@
       <c r="K230" s="39"/>
       <c r="L230" s="39"/>
       <c r="M230" s="40"/>
-      <c r="N230" s="69"/>
-      <c r="O230" s="69"/>
-      <c r="P230" s="69"/>
-      <c r="Q230" s="69"/>
-      <c r="R230" s="69"/>
+      <c r="N230" s="70"/>
+      <c r="O230" s="70"/>
+      <c r="P230" s="70"/>
+      <c r="Q230" s="70"/>
+      <c r="R230" s="70"/>
       <c r="S230" s="49"/>
       <c r="T230" s="41"/>
       <c r="U230" s="41"/>
@@ -8425,7 +8632,7 @@
       <c r="Z230" s="9"/>
     </row>
     <row r="231" spans="1:26" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A231" s="55">
+      <c r="A231" s="56">
         <v>1.1200000000000001</v>
       </c>
       <c r="B231" s="5" t="s">
@@ -8433,25 +8640,27 @@
       </c>
       <c r="C231" s="5"/>
       <c r="D231" s="5"/>
-      <c r="E231" s="56" t="s">
+      <c r="E231" s="57" t="s">
         <v>105</v>
       </c>
       <c r="F231" s="11"/>
       <c r="G231" s="11"/>
       <c r="H231" s="11"/>
       <c r="I231" s="11"/>
-      <c r="J231" s="52"/>
-      <c r="K231" s="53"/>
-      <c r="L231" s="53"/>
-      <c r="M231" s="53"/>
-      <c r="N231" s="71" t="s">
+      <c r="J231" s="53" t="s">
+        <v>100</v>
+      </c>
+      <c r="K231" s="54"/>
+      <c r="L231" s="54"/>
+      <c r="M231" s="54"/>
+      <c r="N231" s="72" t="s">
         <v>106</v>
       </c>
-      <c r="O231" s="72"/>
-      <c r="P231" s="72"/>
-      <c r="Q231" s="72"/>
-      <c r="R231" s="73"/>
-      <c r="S231" s="67" t="s">
+      <c r="O231" s="73"/>
+      <c r="P231" s="73"/>
+      <c r="Q231" s="73"/>
+      <c r="R231" s="74"/>
+      <c r="S231" s="68" t="s">
         <v>41</v>
       </c>
       <c r="T231" s="47"/>
@@ -8467,7 +8676,7 @@
       <c r="B232" s="6"/>
       <c r="C232" s="6"/>
       <c r="D232" s="6"/>
-      <c r="E232" s="57"/>
+      <c r="E232" s="58"/>
       <c r="F232" s="9"/>
       <c r="G232" s="9"/>
       <c r="H232" s="9"/>
@@ -8476,12 +8685,12 @@
       <c r="K232" s="36"/>
       <c r="L232" s="36"/>
       <c r="M232" s="36"/>
-      <c r="N232" s="74"/>
-      <c r="O232" s="70"/>
-      <c r="P232" s="70"/>
-      <c r="Q232" s="70"/>
-      <c r="R232" s="75"/>
-      <c r="S232" s="68"/>
+      <c r="N232" s="75"/>
+      <c r="O232" s="71"/>
+      <c r="P232" s="71"/>
+      <c r="Q232" s="71"/>
+      <c r="R232" s="76"/>
+      <c r="S232" s="69"/>
       <c r="T232" s="41"/>
       <c r="U232" s="41"/>
       <c r="V232" s="41"/>
@@ -8495,7 +8704,7 @@
       <c r="B233" s="7"/>
       <c r="C233" s="7"/>
       <c r="D233" s="7"/>
-      <c r="E233" s="57"/>
+      <c r="E233" s="58"/>
       <c r="F233" s="9"/>
       <c r="G233" s="9"/>
       <c r="H233" s="9"/>
@@ -8504,12 +8713,12 @@
       <c r="K233" s="39"/>
       <c r="L233" s="39"/>
       <c r="M233" s="39"/>
-      <c r="N233" s="76"/>
-      <c r="O233" s="77"/>
-      <c r="P233" s="77"/>
-      <c r="Q233" s="77"/>
-      <c r="R233" s="78"/>
-      <c r="S233" s="68"/>
+      <c r="N233" s="77"/>
+      <c r="O233" s="78"/>
+      <c r="P233" s="78"/>
+      <c r="Q233" s="78"/>
+      <c r="R233" s="79"/>
+      <c r="S233" s="69"/>
       <c r="T233" s="41"/>
       <c r="U233" s="41"/>
       <c r="V233" s="41"/>
@@ -8519,7 +8728,7 @@
       <c r="Z233" s="9"/>
     </row>
     <row r="234" spans="1:26" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A234" s="55">
+      <c r="A234" s="56">
         <v>1.1299999999999999</v>
       </c>
       <c r="B234" s="5" t="s">
@@ -8527,25 +8736,27 @@
       </c>
       <c r="C234" s="5"/>
       <c r="D234" s="5"/>
-      <c r="E234" s="56" t="s">
+      <c r="E234" s="57" t="s">
         <v>108</v>
       </c>
       <c r="F234" s="11"/>
       <c r="G234" s="11"/>
       <c r="H234" s="11"/>
       <c r="I234" s="11"/>
-      <c r="J234" s="52"/>
-      <c r="K234" s="53"/>
-      <c r="L234" s="53"/>
-      <c r="M234" s="53"/>
-      <c r="N234" s="71" t="s">
+      <c r="J234" s="53" t="s">
+        <v>153</v>
+      </c>
+      <c r="K234" s="54"/>
+      <c r="L234" s="54"/>
+      <c r="M234" s="54"/>
+      <c r="N234" s="72" t="s">
         <v>109</v>
       </c>
-      <c r="O234" s="72"/>
-      <c r="P234" s="72"/>
-      <c r="Q234" s="72"/>
-      <c r="R234" s="73"/>
-      <c r="S234" s="67" t="s">
+      <c r="O234" s="73"/>
+      <c r="P234" s="73"/>
+      <c r="Q234" s="73"/>
+      <c r="R234" s="74"/>
+      <c r="S234" s="68" t="s">
         <v>41</v>
       </c>
       <c r="T234" s="47"/>
@@ -8561,7 +8772,7 @@
       <c r="B235" s="6"/>
       <c r="C235" s="6"/>
       <c r="D235" s="6"/>
-      <c r="E235" s="57"/>
+      <c r="E235" s="58"/>
       <c r="F235" s="9"/>
       <c r="G235" s="9"/>
       <c r="H235" s="9"/>
@@ -8570,12 +8781,12 @@
       <c r="K235" s="36"/>
       <c r="L235" s="36"/>
       <c r="M235" s="36"/>
-      <c r="N235" s="74"/>
-      <c r="O235" s="70"/>
-      <c r="P235" s="70"/>
-      <c r="Q235" s="70"/>
-      <c r="R235" s="75"/>
-      <c r="S235" s="68"/>
+      <c r="N235" s="75"/>
+      <c r="O235" s="71"/>
+      <c r="P235" s="71"/>
+      <c r="Q235" s="71"/>
+      <c r="R235" s="76"/>
+      <c r="S235" s="69"/>
       <c r="T235" s="41"/>
       <c r="U235" s="41"/>
       <c r="V235" s="41"/>
@@ -8589,7 +8800,7 @@
       <c r="B236" s="7"/>
       <c r="C236" s="7"/>
       <c r="D236" s="7"/>
-      <c r="E236" s="57"/>
+      <c r="E236" s="58"/>
       <c r="F236" s="9"/>
       <c r="G236" s="9"/>
       <c r="H236" s="9"/>
@@ -8598,12 +8809,12 @@
       <c r="K236" s="39"/>
       <c r="L236" s="39"/>
       <c r="M236" s="39"/>
-      <c r="N236" s="76"/>
-      <c r="O236" s="77"/>
-      <c r="P236" s="77"/>
-      <c r="Q236" s="77"/>
-      <c r="R236" s="78"/>
-      <c r="S236" s="68"/>
+      <c r="N236" s="77"/>
+      <c r="O236" s="78"/>
+      <c r="P236" s="78"/>
+      <c r="Q236" s="78"/>
+      <c r="R236" s="79"/>
+      <c r="S236" s="69"/>
       <c r="T236" s="41"/>
       <c r="U236" s="41"/>
       <c r="V236" s="41"/>
@@ -8613,7 +8824,7 @@
       <c r="Z236" s="9"/>
     </row>
     <row r="237" spans="1:26" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A237" s="55">
+      <c r="A237" s="56">
         <v>1.1399999999999999</v>
       </c>
       <c r="B237" s="5" t="s">
@@ -8621,27 +8832,27 @@
       </c>
       <c r="C237" s="5"/>
       <c r="D237" s="5"/>
-      <c r="E237" s="56" t="s">
+      <c r="E237" s="57" t="s">
         <v>117</v>
       </c>
       <c r="F237" s="11"/>
       <c r="G237" s="11"/>
       <c r="H237" s="11"/>
       <c r="I237" s="11"/>
-      <c r="J237" s="52" t="s">
+      <c r="J237" s="53" t="s">
         <v>111</v>
       </c>
-      <c r="K237" s="53"/>
-      <c r="L237" s="53"/>
-      <c r="M237" s="53"/>
-      <c r="N237" s="71" t="s">
+      <c r="K237" s="54"/>
+      <c r="L237" s="54"/>
+      <c r="M237" s="54"/>
+      <c r="N237" s="72" t="s">
         <v>112</v>
       </c>
-      <c r="O237" s="72"/>
-      <c r="P237" s="72"/>
-      <c r="Q237" s="72"/>
-      <c r="R237" s="73"/>
-      <c r="S237" s="67" t="s">
+      <c r="O237" s="73"/>
+      <c r="P237" s="73"/>
+      <c r="Q237" s="73"/>
+      <c r="R237" s="74"/>
+      <c r="S237" s="68" t="s">
         <v>41</v>
       </c>
       <c r="T237" s="47"/>
@@ -8657,7 +8868,7 @@
       <c r="B238" s="6"/>
       <c r="C238" s="6"/>
       <c r="D238" s="6"/>
-      <c r="E238" s="57"/>
+      <c r="E238" s="58"/>
       <c r="F238" s="9"/>
       <c r="G238" s="9"/>
       <c r="H238" s="9"/>
@@ -8666,12 +8877,12 @@
       <c r="K238" s="36"/>
       <c r="L238" s="36"/>
       <c r="M238" s="36"/>
-      <c r="N238" s="74"/>
-      <c r="O238" s="70"/>
-      <c r="P238" s="70"/>
-      <c r="Q238" s="70"/>
-      <c r="R238" s="75"/>
-      <c r="S238" s="68"/>
+      <c r="N238" s="75"/>
+      <c r="O238" s="71"/>
+      <c r="P238" s="71"/>
+      <c r="Q238" s="71"/>
+      <c r="R238" s="76"/>
+      <c r="S238" s="69"/>
       <c r="T238" s="41"/>
       <c r="U238" s="41"/>
       <c r="V238" s="41"/>
@@ -8685,7 +8896,7 @@
       <c r="B239" s="7"/>
       <c r="C239" s="7"/>
       <c r="D239" s="7"/>
-      <c r="E239" s="57"/>
+      <c r="E239" s="58"/>
       <c r="F239" s="9"/>
       <c r="G239" s="9"/>
       <c r="H239" s="9"/>
@@ -8694,12 +8905,12 @@
       <c r="K239" s="39"/>
       <c r="L239" s="39"/>
       <c r="M239" s="39"/>
-      <c r="N239" s="76"/>
-      <c r="O239" s="77"/>
-      <c r="P239" s="77"/>
-      <c r="Q239" s="77"/>
-      <c r="R239" s="78"/>
-      <c r="S239" s="68"/>
+      <c r="N239" s="77"/>
+      <c r="O239" s="78"/>
+      <c r="P239" s="78"/>
+      <c r="Q239" s="78"/>
+      <c r="R239" s="79"/>
+      <c r="S239" s="69"/>
       <c r="T239" s="41"/>
       <c r="U239" s="41"/>
       <c r="V239" s="41"/>
@@ -8709,7 +8920,7 @@
       <c r="Z239" s="9"/>
     </row>
     <row r="240" spans="1:26" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A240" s="55">
+      <c r="A240" s="56">
         <v>1.1499999999999999</v>
       </c>
       <c r="B240" s="5" t="s">
@@ -8720,24 +8931,24 @@
       <c r="E240" s="18" t="s">
         <v>118</v>
       </c>
-      <c r="F240" s="60"/>
-      <c r="G240" s="60"/>
-      <c r="H240" s="60"/>
-      <c r="I240" s="61"/>
-      <c r="J240" s="52" t="s">
+      <c r="F240" s="61"/>
+      <c r="G240" s="61"/>
+      <c r="H240" s="61"/>
+      <c r="I240" s="62"/>
+      <c r="J240" s="53" t="s">
         <v>114</v>
       </c>
-      <c r="K240" s="53"/>
-      <c r="L240" s="53"/>
-      <c r="M240" s="53"/>
-      <c r="N240" s="71" t="s">
+      <c r="K240" s="54"/>
+      <c r="L240" s="54"/>
+      <c r="M240" s="54"/>
+      <c r="N240" s="72" t="s">
         <v>115</v>
       </c>
-      <c r="O240" s="72"/>
-      <c r="P240" s="72"/>
-      <c r="Q240" s="72"/>
-      <c r="R240" s="73"/>
-      <c r="S240" s="67" t="s">
+      <c r="O240" s="73"/>
+      <c r="P240" s="73"/>
+      <c r="Q240" s="73"/>
+      <c r="R240" s="74"/>
+      <c r="S240" s="68" t="s">
         <v>41</v>
       </c>
       <c r="T240" s="47"/>
@@ -8753,21 +8964,21 @@
       <c r="B241" s="6"/>
       <c r="C241" s="6"/>
       <c r="D241" s="6"/>
-      <c r="E241" s="62"/>
-      <c r="F241" s="63"/>
-      <c r="G241" s="63"/>
-      <c r="H241" s="63"/>
-      <c r="I241" s="64"/>
+      <c r="E241" s="63"/>
+      <c r="F241" s="64"/>
+      <c r="G241" s="64"/>
+      <c r="H241" s="64"/>
+      <c r="I241" s="65"/>
       <c r="J241" s="35"/>
       <c r="K241" s="36"/>
       <c r="L241" s="36"/>
       <c r="M241" s="36"/>
-      <c r="N241" s="74"/>
-      <c r="O241" s="70"/>
-      <c r="P241" s="70"/>
-      <c r="Q241" s="70"/>
-      <c r="R241" s="75"/>
-      <c r="S241" s="68"/>
+      <c r="N241" s="75"/>
+      <c r="O241" s="71"/>
+      <c r="P241" s="71"/>
+      <c r="Q241" s="71"/>
+      <c r="R241" s="76"/>
+      <c r="S241" s="69"/>
       <c r="T241" s="41"/>
       <c r="U241" s="41"/>
       <c r="V241" s="41"/>
@@ -8781,21 +8992,21 @@
       <c r="B242" s="7"/>
       <c r="C242" s="7"/>
       <c r="D242" s="7"/>
-      <c r="E242" s="65"/>
-      <c r="F242" s="66"/>
-      <c r="G242" s="66"/>
-      <c r="H242" s="66"/>
-      <c r="I242" s="56"/>
+      <c r="E242" s="66"/>
+      <c r="F242" s="67"/>
+      <c r="G242" s="67"/>
+      <c r="H242" s="67"/>
+      <c r="I242" s="57"/>
       <c r="J242" s="38"/>
       <c r="K242" s="39"/>
       <c r="L242" s="39"/>
       <c r="M242" s="39"/>
-      <c r="N242" s="76"/>
-      <c r="O242" s="77"/>
-      <c r="P242" s="77"/>
-      <c r="Q242" s="77"/>
-      <c r="R242" s="78"/>
-      <c r="S242" s="68"/>
+      <c r="N242" s="77"/>
+      <c r="O242" s="78"/>
+      <c r="P242" s="78"/>
+      <c r="Q242" s="78"/>
+      <c r="R242" s="79"/>
+      <c r="S242" s="69"/>
       <c r="T242" s="41"/>
       <c r="U242" s="41"/>
       <c r="V242" s="41"/>
@@ -8805,7 +9016,7 @@
       <c r="Z242" s="9"/>
     </row>
     <row r="243" spans="1:26" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A243" s="55">
+      <c r="A243" s="56">
         <v>1.1499999999999999</v>
       </c>
       <c r="B243" s="5" t="s">
@@ -8816,24 +9027,24 @@
       <c r="E243" s="18" t="s">
         <v>118</v>
       </c>
-      <c r="F243" s="60"/>
-      <c r="G243" s="60"/>
-      <c r="H243" s="60"/>
-      <c r="I243" s="61"/>
-      <c r="J243" s="52" t="s">
+      <c r="F243" s="61"/>
+      <c r="G243" s="61"/>
+      <c r="H243" s="61"/>
+      <c r="I243" s="62"/>
+      <c r="J243" s="53" t="s">
         <v>119</v>
       </c>
-      <c r="K243" s="53"/>
-      <c r="L243" s="53"/>
-      <c r="M243" s="53"/>
-      <c r="N243" s="71" t="s">
+      <c r="K243" s="54"/>
+      <c r="L243" s="54"/>
+      <c r="M243" s="54"/>
+      <c r="N243" s="72" t="s">
         <v>120</v>
       </c>
-      <c r="O243" s="72"/>
-      <c r="P243" s="72"/>
-      <c r="Q243" s="72"/>
-      <c r="R243" s="73"/>
-      <c r="S243" s="67" t="s">
+      <c r="O243" s="73"/>
+      <c r="P243" s="73"/>
+      <c r="Q243" s="73"/>
+      <c r="R243" s="74"/>
+      <c r="S243" s="68" t="s">
         <v>41</v>
       </c>
       <c r="T243" s="47"/>
@@ -8849,21 +9060,21 @@
       <c r="B244" s="6"/>
       <c r="C244" s="6"/>
       <c r="D244" s="6"/>
-      <c r="E244" s="62"/>
-      <c r="F244" s="63"/>
-      <c r="G244" s="63"/>
-      <c r="H244" s="63"/>
-      <c r="I244" s="64"/>
+      <c r="E244" s="63"/>
+      <c r="F244" s="64"/>
+      <c r="G244" s="64"/>
+      <c r="H244" s="64"/>
+      <c r="I244" s="65"/>
       <c r="J244" s="35"/>
       <c r="K244" s="36"/>
       <c r="L244" s="36"/>
       <c r="M244" s="36"/>
-      <c r="N244" s="74"/>
-      <c r="O244" s="70"/>
-      <c r="P244" s="70"/>
-      <c r="Q244" s="70"/>
-      <c r="R244" s="75"/>
-      <c r="S244" s="68"/>
+      <c r="N244" s="75"/>
+      <c r="O244" s="71"/>
+      <c r="P244" s="71"/>
+      <c r="Q244" s="71"/>
+      <c r="R244" s="76"/>
+      <c r="S244" s="69"/>
       <c r="T244" s="41"/>
       <c r="U244" s="41"/>
       <c r="V244" s="41"/>
@@ -8877,21 +9088,21 @@
       <c r="B245" s="7"/>
       <c r="C245" s="7"/>
       <c r="D245" s="7"/>
-      <c r="E245" s="65"/>
-      <c r="F245" s="66"/>
-      <c r="G245" s="66"/>
-      <c r="H245" s="66"/>
-      <c r="I245" s="56"/>
+      <c r="E245" s="66"/>
+      <c r="F245" s="67"/>
+      <c r="G245" s="67"/>
+      <c r="H245" s="67"/>
+      <c r="I245" s="57"/>
       <c r="J245" s="38"/>
       <c r="K245" s="39"/>
       <c r="L245" s="39"/>
       <c r="M245" s="39"/>
-      <c r="N245" s="76"/>
-      <c r="O245" s="77"/>
-      <c r="P245" s="77"/>
-      <c r="Q245" s="77"/>
-      <c r="R245" s="78"/>
-      <c r="S245" s="68"/>
+      <c r="N245" s="77"/>
+      <c r="O245" s="78"/>
+      <c r="P245" s="78"/>
+      <c r="Q245" s="78"/>
+      <c r="R245" s="79"/>
+      <c r="S245" s="69"/>
       <c r="T245" s="41"/>
       <c r="U245" s="41"/>
       <c r="V245" s="41"/>
@@ -8901,28 +9112,28 @@
       <c r="Z245" s="9"/>
     </row>
     <row r="246" spans="1:26" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A246" s="55">
+      <c r="A246" s="56">
         <v>1.1599999999999999</v>
       </c>
-      <c r="B246" s="52" t="s">
+      <c r="B246" s="53" t="s">
         <v>121</v>
       </c>
-      <c r="C246" s="53"/>
-      <c r="D246" s="54"/>
+      <c r="C246" s="54"/>
+      <c r="D246" s="55"/>
       <c r="E246" s="18" t="s">
         <v>123</v>
       </c>
-      <c r="F246" s="60"/>
-      <c r="G246" s="60"/>
-      <c r="H246" s="60"/>
-      <c r="I246" s="61"/>
-      <c r="J246" s="52" t="s">
+      <c r="F246" s="61"/>
+      <c r="G246" s="61"/>
+      <c r="H246" s="61"/>
+      <c r="I246" s="62"/>
+      <c r="J246" s="53" t="s">
         <v>114</v>
       </c>
-      <c r="K246" s="53"/>
-      <c r="L246" s="53"/>
-      <c r="M246" s="53"/>
-      <c r="N246" s="59" t="s">
+      <c r="K246" s="54"/>
+      <c r="L246" s="54"/>
+      <c r="M246" s="54"/>
+      <c r="N246" s="60" t="s">
         <v>122</v>
       </c>
       <c r="O246" s="47"/>
@@ -8945,11 +9156,11 @@
       <c r="B247" s="35"/>
       <c r="C247" s="36"/>
       <c r="D247" s="37"/>
-      <c r="E247" s="62"/>
-      <c r="F247" s="63"/>
-      <c r="G247" s="63"/>
-      <c r="H247" s="63"/>
-      <c r="I247" s="64"/>
+      <c r="E247" s="63"/>
+      <c r="F247" s="64"/>
+      <c r="G247" s="64"/>
+      <c r="H247" s="64"/>
+      <c r="I247" s="65"/>
       <c r="J247" s="35"/>
       <c r="K247" s="36"/>
       <c r="L247" s="36"/>
@@ -8973,11 +9184,11 @@
       <c r="B248" s="38"/>
       <c r="C248" s="39"/>
       <c r="D248" s="40"/>
-      <c r="E248" s="65"/>
-      <c r="F248" s="66"/>
-      <c r="G248" s="66"/>
-      <c r="H248" s="66"/>
-      <c r="I248" s="56"/>
+      <c r="E248" s="66"/>
+      <c r="F248" s="67"/>
+      <c r="G248" s="67"/>
+      <c r="H248" s="67"/>
+      <c r="I248" s="57"/>
       <c r="J248" s="38"/>
       <c r="K248" s="39"/>
       <c r="L248" s="39"/>
@@ -8997,7 +9208,7 @@
       <c r="Z248" s="9"/>
     </row>
     <row r="249" spans="1:26" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A249" s="55">
+      <c r="A249" s="56">
         <v>1.17</v>
       </c>
       <c r="B249" s="5" t="s">
@@ -9005,27 +9216,27 @@
       </c>
       <c r="C249" s="5"/>
       <c r="D249" s="5"/>
-      <c r="E249" s="56" t="s">
+      <c r="E249" s="57" t="s">
         <v>124</v>
       </c>
       <c r="F249" s="11"/>
       <c r="G249" s="11"/>
       <c r="H249" s="11"/>
       <c r="I249" s="11"/>
-      <c r="J249" s="52" t="s">
+      <c r="J249" s="53" t="s">
         <v>114</v>
       </c>
-      <c r="K249" s="53"/>
-      <c r="L249" s="53"/>
-      <c r="M249" s="53"/>
-      <c r="N249" s="71" t="s">
+      <c r="K249" s="54"/>
+      <c r="L249" s="54"/>
+      <c r="M249" s="54"/>
+      <c r="N249" s="72" t="s">
         <v>125</v>
       </c>
-      <c r="O249" s="72"/>
-      <c r="P249" s="72"/>
-      <c r="Q249" s="72"/>
-      <c r="R249" s="73"/>
-      <c r="S249" s="67" t="s">
+      <c r="O249" s="73"/>
+      <c r="P249" s="73"/>
+      <c r="Q249" s="73"/>
+      <c r="R249" s="74"/>
+      <c r="S249" s="68" t="s">
         <v>41</v>
       </c>
       <c r="T249" s="47"/>
@@ -9041,7 +9252,7 @@
       <c r="B250" s="6"/>
       <c r="C250" s="6"/>
       <c r="D250" s="6"/>
-      <c r="E250" s="57"/>
+      <c r="E250" s="58"/>
       <c r="F250" s="9"/>
       <c r="G250" s="9"/>
       <c r="H250" s="9"/>
@@ -9050,12 +9261,12 @@
       <c r="K250" s="36"/>
       <c r="L250" s="36"/>
       <c r="M250" s="36"/>
-      <c r="N250" s="74"/>
-      <c r="O250" s="70"/>
-      <c r="P250" s="70"/>
-      <c r="Q250" s="70"/>
-      <c r="R250" s="75"/>
-      <c r="S250" s="68"/>
+      <c r="N250" s="75"/>
+      <c r="O250" s="71"/>
+      <c r="P250" s="71"/>
+      <c r="Q250" s="71"/>
+      <c r="R250" s="76"/>
+      <c r="S250" s="69"/>
       <c r="T250" s="41"/>
       <c r="U250" s="41"/>
       <c r="V250" s="41"/>
@@ -9069,7 +9280,7 @@
       <c r="B251" s="7"/>
       <c r="C251" s="7"/>
       <c r="D251" s="7"/>
-      <c r="E251" s="57"/>
+      <c r="E251" s="58"/>
       <c r="F251" s="9"/>
       <c r="G251" s="9"/>
       <c r="H251" s="9"/>
@@ -9078,12 +9289,12 @@
       <c r="K251" s="39"/>
       <c r="L251" s="39"/>
       <c r="M251" s="39"/>
-      <c r="N251" s="76"/>
-      <c r="O251" s="77"/>
-      <c r="P251" s="77"/>
-      <c r="Q251" s="77"/>
-      <c r="R251" s="78"/>
-      <c r="S251" s="68"/>
+      <c r="N251" s="77"/>
+      <c r="O251" s="78"/>
+      <c r="P251" s="78"/>
+      <c r="Q251" s="78"/>
+      <c r="R251" s="79"/>
+      <c r="S251" s="69"/>
       <c r="T251" s="41"/>
       <c r="U251" s="41"/>
       <c r="V251" s="41"/>
@@ -9093,7 +9304,7 @@
       <c r="Z251" s="9"/>
     </row>
     <row r="252" spans="1:26" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A252" s="55">
+      <c r="A252" s="56">
         <v>1.18</v>
       </c>
       <c r="B252" s="5" t="s">
@@ -9101,27 +9312,27 @@
       </c>
       <c r="C252" s="5"/>
       <c r="D252" s="5"/>
-      <c r="E252" s="56" t="s">
+      <c r="E252" s="57" t="s">
         <v>129</v>
       </c>
       <c r="F252" s="11"/>
       <c r="G252" s="11"/>
       <c r="H252" s="11"/>
       <c r="I252" s="11"/>
-      <c r="J252" s="52" t="s">
+      <c r="J252" s="53" t="s">
         <v>42</v>
       </c>
-      <c r="K252" s="53"/>
-      <c r="L252" s="53"/>
-      <c r="M252" s="53"/>
-      <c r="N252" s="71" t="s">
+      <c r="K252" s="54"/>
+      <c r="L252" s="54"/>
+      <c r="M252" s="54"/>
+      <c r="N252" s="72" t="s">
         <v>128</v>
       </c>
-      <c r="O252" s="72"/>
-      <c r="P252" s="72"/>
-      <c r="Q252" s="72"/>
-      <c r="R252" s="73"/>
-      <c r="S252" s="67" t="s">
+      <c r="O252" s="73"/>
+      <c r="P252" s="73"/>
+      <c r="Q252" s="73"/>
+      <c r="R252" s="74"/>
+      <c r="S252" s="68" t="s">
         <v>41</v>
       </c>
       <c r="T252" s="47"/>
@@ -9137,7 +9348,7 @@
       <c r="B253" s="6"/>
       <c r="C253" s="6"/>
       <c r="D253" s="6"/>
-      <c r="E253" s="57"/>
+      <c r="E253" s="58"/>
       <c r="F253" s="9"/>
       <c r="G253" s="9"/>
       <c r="H253" s="9"/>
@@ -9146,12 +9357,12 @@
       <c r="K253" s="36"/>
       <c r="L253" s="36"/>
       <c r="M253" s="36"/>
-      <c r="N253" s="74"/>
-      <c r="O253" s="70"/>
-      <c r="P253" s="70"/>
-      <c r="Q253" s="70"/>
-      <c r="R253" s="75"/>
-      <c r="S253" s="68"/>
+      <c r="N253" s="75"/>
+      <c r="O253" s="71"/>
+      <c r="P253" s="71"/>
+      <c r="Q253" s="71"/>
+      <c r="R253" s="76"/>
+      <c r="S253" s="69"/>
       <c r="T253" s="41"/>
       <c r="U253" s="41"/>
       <c r="V253" s="41"/>
@@ -9165,7 +9376,7 @@
       <c r="B254" s="7"/>
       <c r="C254" s="7"/>
       <c r="D254" s="7"/>
-      <c r="E254" s="57"/>
+      <c r="E254" s="58"/>
       <c r="F254" s="9"/>
       <c r="G254" s="9"/>
       <c r="H254" s="9"/>
@@ -9174,12 +9385,12 @@
       <c r="K254" s="39"/>
       <c r="L254" s="39"/>
       <c r="M254" s="39"/>
-      <c r="N254" s="76"/>
-      <c r="O254" s="77"/>
-      <c r="P254" s="77"/>
-      <c r="Q254" s="77"/>
-      <c r="R254" s="78"/>
-      <c r="S254" s="68"/>
+      <c r="N254" s="77"/>
+      <c r="O254" s="78"/>
+      <c r="P254" s="78"/>
+      <c r="Q254" s="78"/>
+      <c r="R254" s="79"/>
+      <c r="S254" s="69"/>
       <c r="T254" s="41"/>
       <c r="U254" s="41"/>
       <c r="V254" s="41"/>
@@ -9189,7 +9400,7 @@
       <c r="Z254" s="9"/>
     </row>
     <row r="255" spans="1:26" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A255" s="55">
+      <c r="A255" s="56">
         <v>1.19</v>
       </c>
       <c r="B255" s="5" t="s">
@@ -9197,27 +9408,27 @@
       </c>
       <c r="C255" s="5"/>
       <c r="D255" s="5"/>
-      <c r="E255" s="56" t="s">
+      <c r="E255" s="57" t="s">
         <v>131</v>
       </c>
       <c r="F255" s="11"/>
       <c r="G255" s="11"/>
       <c r="H255" s="11"/>
       <c r="I255" s="11"/>
-      <c r="J255" s="52" t="s">
+      <c r="J255" s="53" t="s">
         <v>132</v>
       </c>
-      <c r="K255" s="53"/>
-      <c r="L255" s="53"/>
-      <c r="M255" s="53"/>
-      <c r="N255" s="71" t="s">
+      <c r="K255" s="54"/>
+      <c r="L255" s="54"/>
+      <c r="M255" s="54"/>
+      <c r="N255" s="72" t="s">
         <v>133</v>
       </c>
-      <c r="O255" s="72"/>
-      <c r="P255" s="72"/>
-      <c r="Q255" s="72"/>
-      <c r="R255" s="73"/>
-      <c r="S255" s="67" t="s">
+      <c r="O255" s="73"/>
+      <c r="P255" s="73"/>
+      <c r="Q255" s="73"/>
+      <c r="R255" s="74"/>
+      <c r="S255" s="68" t="s">
         <v>41</v>
       </c>
       <c r="T255" s="47"/>
@@ -9233,7 +9444,7 @@
       <c r="B256" s="6"/>
       <c r="C256" s="6"/>
       <c r="D256" s="6"/>
-      <c r="E256" s="57"/>
+      <c r="E256" s="58"/>
       <c r="F256" s="9"/>
       <c r="G256" s="9"/>
       <c r="H256" s="9"/>
@@ -9242,12 +9453,12 @@
       <c r="K256" s="36"/>
       <c r="L256" s="36"/>
       <c r="M256" s="36"/>
-      <c r="N256" s="74"/>
-      <c r="O256" s="70"/>
-      <c r="P256" s="70"/>
-      <c r="Q256" s="70"/>
-      <c r="R256" s="75"/>
-      <c r="S256" s="68"/>
+      <c r="N256" s="75"/>
+      <c r="O256" s="71"/>
+      <c r="P256" s="71"/>
+      <c r="Q256" s="71"/>
+      <c r="R256" s="76"/>
+      <c r="S256" s="69"/>
       <c r="T256" s="41"/>
       <c r="U256" s="41"/>
       <c r="V256" s="41"/>
@@ -9261,7 +9472,7 @@
       <c r="B257" s="7"/>
       <c r="C257" s="7"/>
       <c r="D257" s="7"/>
-      <c r="E257" s="57"/>
+      <c r="E257" s="58"/>
       <c r="F257" s="9"/>
       <c r="G257" s="9"/>
       <c r="H257" s="9"/>
@@ -9270,12 +9481,12 @@
       <c r="K257" s="39"/>
       <c r="L257" s="39"/>
       <c r="M257" s="39"/>
-      <c r="N257" s="76"/>
-      <c r="O257" s="77"/>
-      <c r="P257" s="77"/>
-      <c r="Q257" s="77"/>
-      <c r="R257" s="78"/>
-      <c r="S257" s="68"/>
+      <c r="N257" s="77"/>
+      <c r="O257" s="78"/>
+      <c r="P257" s="78"/>
+      <c r="Q257" s="78"/>
+      <c r="R257" s="79"/>
+      <c r="S257" s="69"/>
       <c r="T257" s="41"/>
       <c r="U257" s="41"/>
       <c r="V257" s="41"/>
@@ -9284,8 +9495,104 @@
       <c r="Y257" s="9"/>
       <c r="Z257" s="9"/>
     </row>
+    <row r="258" spans="1:26" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A258" s="56">
+        <v>1.2</v>
+      </c>
+      <c r="B258" s="5" t="s">
+        <v>134</v>
+      </c>
+      <c r="C258" s="5"/>
+      <c r="D258" s="5"/>
+      <c r="E258" s="57" t="s">
+        <v>135</v>
+      </c>
+      <c r="F258" s="11"/>
+      <c r="G258" s="11"/>
+      <c r="H258" s="11"/>
+      <c r="I258" s="11"/>
+      <c r="J258" s="53" t="s">
+        <v>100</v>
+      </c>
+      <c r="K258" s="54"/>
+      <c r="L258" s="54"/>
+      <c r="M258" s="55"/>
+      <c r="N258" s="52" t="s">
+        <v>136</v>
+      </c>
+      <c r="O258" s="41"/>
+      <c r="P258" s="41"/>
+      <c r="Q258" s="41"/>
+      <c r="R258" s="41"/>
+      <c r="S258" s="48" t="s">
+        <v>41</v>
+      </c>
+      <c r="T258" s="47"/>
+      <c r="U258" s="47"/>
+      <c r="V258" s="47"/>
+      <c r="W258" s="47"/>
+      <c r="X258" s="11"/>
+      <c r="Y258" s="11"/>
+      <c r="Z258" s="11"/>
+    </row>
+    <row r="259" spans="1:26" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A259" s="50"/>
+      <c r="B259" s="6"/>
+      <c r="C259" s="6"/>
+      <c r="D259" s="6"/>
+      <c r="E259" s="58"/>
+      <c r="F259" s="9"/>
+      <c r="G259" s="9"/>
+      <c r="H259" s="9"/>
+      <c r="I259" s="9"/>
+      <c r="J259" s="35"/>
+      <c r="K259" s="36"/>
+      <c r="L259" s="36"/>
+      <c r="M259" s="37"/>
+      <c r="N259" s="41"/>
+      <c r="O259" s="41"/>
+      <c r="P259" s="41"/>
+      <c r="Q259" s="41"/>
+      <c r="R259" s="41"/>
+      <c r="S259" s="49"/>
+      <c r="T259" s="41"/>
+      <c r="U259" s="41"/>
+      <c r="V259" s="41"/>
+      <c r="W259" s="41"/>
+      <c r="X259" s="9"/>
+      <c r="Y259" s="9"/>
+      <c r="Z259" s="9"/>
+    </row>
+    <row r="260" spans="1:26" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A260" s="51"/>
+      <c r="B260" s="7"/>
+      <c r="C260" s="7"/>
+      <c r="D260" s="7"/>
+      <c r="E260" s="58"/>
+      <c r="F260" s="9"/>
+      <c r="G260" s="9"/>
+      <c r="H260" s="9"/>
+      <c r="I260" s="9"/>
+      <c r="J260" s="38"/>
+      <c r="K260" s="39"/>
+      <c r="L260" s="39"/>
+      <c r="M260" s="40"/>
+      <c r="N260" s="41"/>
+      <c r="O260" s="41"/>
+      <c r="P260" s="41"/>
+      <c r="Q260" s="41"/>
+      <c r="R260" s="41"/>
+      <c r="S260" s="49"/>
+      <c r="T260" s="41"/>
+      <c r="U260" s="41"/>
+      <c r="V260" s="41"/>
+      <c r="W260" s="41"/>
+      <c r="X260" s="9"/>
+      <c r="Y260" s="9"/>
+      <c r="Z260" s="9"/>
+    </row>
   </sheetData>
-  <mergeCells count="557">
+  <mergeCells count="565">
     <mergeCell ref="A255:A257"/>
     <mergeCell ref="B255:D257"/>
     <mergeCell ref="E255:I257"/>
@@ -9294,6 +9601,14 @@
     <mergeCell ref="S255:S257"/>
     <mergeCell ref="T255:W257"/>
     <mergeCell ref="X255:Z257"/>
+    <mergeCell ref="A258:A260"/>
+    <mergeCell ref="B258:D260"/>
+    <mergeCell ref="E258:I260"/>
+    <mergeCell ref="J258:M260"/>
+    <mergeCell ref="N258:R260"/>
+    <mergeCell ref="S258:S260"/>
+    <mergeCell ref="T258:W260"/>
+    <mergeCell ref="X258:Z260"/>
     <mergeCell ref="N249:R251"/>
     <mergeCell ref="S249:S251"/>
     <mergeCell ref="T249:W251"/>

</xml_diff>